<commit_message>
added the UML for the M8
</commit_message>
<xml_diff>
--- a/Presentation/Budget.xlsx
+++ b/Presentation/Budget.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Amount</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Female to Female Breadboard Wire</t>
+  </si>
+  <si>
+    <t>16Gb SD Card</t>
   </si>
 </sst>
 </file>
@@ -305,11 +308,28 @@
               <a:effectLst/>
             </c:spPr>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$2:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Raspberry Pi Model B+</c:v>
                 </c:pt>
@@ -331,15 +351,18 @@
                 <c:pt idx="6">
                   <c:v>Female to Female Breadboard Wire</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>16Gb SD Card</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:f>Sheet1!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>119.85000000000001</c:v>
                 </c:pt>
@@ -360,6 +383,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>6.82</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29.97</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1313,7 +1339,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1358,7 +1384,7 @@
       </c>
       <c r="F2" s="2">
         <f>SUM(D2:D200)</f>
-        <v>607.96</v>
+        <v>637.93000000000006</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1452,9 +1478,18 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>9.99</v>
+      </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>29.97</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added the budget for the master node
</commit_message>
<xml_diff>
--- a/Presentation/Budget.xlsx
+++ b/Presentation/Budget.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silas\Documents\GitHub\driftNode\Presentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Users\Silas Rubinson\Documents\GitHub\driftNode\Presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Amount</t>
   </si>
@@ -53,9 +53,6 @@
     <t>NVIDIA Jetson tk1</t>
   </si>
   <si>
-    <t>Items current</t>
-  </si>
-  <si>
     <t>Weller WES51 Soldering Station</t>
   </si>
   <si>
@@ -63,6 +60,30 @@
   </si>
   <si>
     <t>16Gb SD Card</t>
+  </si>
+  <si>
+    <t>X-IMU</t>
+  </si>
+  <si>
+    <t>NETIS WF-2116 N300 Wi-Fi</t>
+  </si>
+  <si>
+    <t>GPS Antenna</t>
+  </si>
+  <si>
+    <t>Rraspberry PI Camera Board</t>
+  </si>
+  <si>
+    <t>Smal Node</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>32Gb SD Card</t>
+  </si>
+  <si>
+    <t>Master Node</t>
   </si>
 </sst>
 </file>
@@ -325,11 +346,104 @@
               <a:effectLst/>
             </c:spPr>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$1:$A$20</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$A$2:$A$7,Sheet1!$A$11:$A$16,Sheet1!$A$19:$A$20)</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Raspberry Pi Model B+</c:v>
                 </c:pt>
@@ -343,53 +457,143 @@
                   <c:v>MinIMU-9 v3</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>16Gb SD Card</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Rraspberry PI Camera Board</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>NVIDIA Jetson tk1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>Adafruit Ultimate GPS</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>X-IMU</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>NETIS WF-2116 N300 Wi-Fi</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>GPS Antenna</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32Gb SD Card</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Weller WES51 Soldering Station</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="13">
                   <c:v>Female to Female Breadboard Wire</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16Gb SD Card</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$9</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$D$2:$D$20</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$D$3:$D$8,Sheet1!$D$12:$D$17,Sheet1!$D$20)</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>119.85000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>119.85000000000001</c:v>
+                  <c:v>26.099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.099999999999998</c:v>
+                  <c:v>59.849999999999994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>59.849999999999994</c:v>
+                  <c:v>29.97</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>192.99</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>82.5</c:v>
+                  <c:v>89.85</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>39.950000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400.57</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19.989999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.95</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.69</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>6.82</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>29.97</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:categoryFilterExceptions>
+                <c15:categoryFilterException>
+                  <c15:sqref>Sheet1!$D$2</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+                <c15:categoryFilterException>
+                  <c15:sqref>Sheet1!$D$11</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+                <c15:categoryFilterException>
+                  <c15:sqref>Sheet1!$D$19</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6">
+                        <a:lumMod val="80000"/>
+                        <a:lumOff val="20000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+              </c15:categoryFilterExceptions>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -426,6 +630,683 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr rtl="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Master Node</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$10:$A$16</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$11:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>NVIDIA Jetson tk1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Adafruit Ultimate GPS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>X-IMU</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>NETIS WF-2116 N300 Wi-Fi</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>GPS Antenna</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32Gb SD Card</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$10:$B$16</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$11:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:categoryFilterExceptions/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredPieSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:dPt>
+                  <c:idx val="0"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="1"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="2"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="3"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="4"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="5"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Sheet1!$A$10:$A$16</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$11:$A$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>NVIDIA Jetson tk1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Adafruit Ultimate GPS</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>X-IMU</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>NETIS WF-2116 N300 Wi-Fi</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>GPS Antenna</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>32Gb SD Card</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Sheet1!$C$10:$C$16</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$11:$C$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>192.99</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>39.950000000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>400.57</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>19.989999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>12.95</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>15.69</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                    <c15:categoryFilterExceptions/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredPieSeries>
+            <c15:filteredPieSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:dPt>
+                  <c:idx val="0"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="1"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="2"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="3"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="4"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="5"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Sheet1!$A$10:$A$16</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$11:$A$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>NVIDIA Jetson tk1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Adafruit Ultimate GPS</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>X-IMU</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>NETIS WF-2116 N300 Wi-Fi</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>GPS Antenna</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>32Gb SD Card</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Sheet1!$D$10:$D$16</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$D$11:$D$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>192.99</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>39.950000000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>400.57</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>19.989999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>12.95</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>15.69</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                    <c15:categoryFilterExceptions/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredPieSeries>
+          </c:ext>
+        </c:extLst>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -519,7 +1400,566 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1043,15 +2483,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:colOff>523874</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:rowOff>70484</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1065,6 +2505,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1336,23 +2806,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A10" sqref="A10:D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1368,7 +2838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1383,11 +2853,11 @@
         <v>119.85000000000001</v>
       </c>
       <c r="F2" s="2">
-        <f>SUM(D2:D200)</f>
-        <v>637.93000000000006</v>
+        <f>SUM(D2:D196)</f>
+        <v>1899.0700000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1398,11 +2868,11 @@
         <v>39.950000000000003</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D28" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D24" si="0">B3*C3</f>
         <v>119.85000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1417,7 +2887,7 @@
         <v>26.099999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1432,179 +2902,194 @@
         <v>59.849999999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1">
-        <v>192.99</v>
+        <v>9.99</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>192.99</v>
+        <v>29.97</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1">
-        <v>82.5</v>
+        <v>29.95</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>82.5</v>
+        <v>89.85</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" s="1">
-        <v>3.41</v>
-      </c>
-      <c r="D8" s="1">
-        <f t="shared" si="0"/>
-        <v>6.82</v>
-      </c>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <f>SUM(D11:D16)</f>
+        <v>682.1400000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>192.99</v>
+      </c>
+      <c r="D11" s="1">
+        <f>B11*C11</f>
+        <v>192.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" ref="D12" si="1">B12*C12</f>
+        <v>39.950000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1">
-        <v>9.99</v>
-      </c>
-      <c r="D9" s="1">
-        <f t="shared" si="0"/>
-        <v>29.97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D10" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D11" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D12" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>400.57</v>
+      </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>400.57</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>19.989999999999998</v>
+      </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>19.989999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>12.95</v>
+      </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12.95</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <v>15.69</v>
+      </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15.69</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D17" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D18" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1">
+        <v>82.5</v>
+      </c>
       <c r="D19" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>B19*C19</f>
+        <v>82.5</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3.41</v>
+      </c>
       <c r="D20" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>B20*C20</f>
+        <v>6.82</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D21" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D22" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D23" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D24" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D25" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D26" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D27" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D28" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added more budget stuff for the master node
</commit_message>
<xml_diff>
--- a/Presentation/Budget.xlsx
+++ b/Presentation/Budget.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Amount</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>Master Node</t>
+  </si>
+  <si>
+    <t>Node Casing</t>
+  </si>
+  <si>
+    <t>Xbee</t>
+  </si>
+  <si>
+    <t>Battery</t>
   </si>
 </sst>
 </file>
@@ -432,18 +441,72 @@
               <a:effectLst/>
             </c:spPr>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$A$1:$A$20</c15:sqref>
+                    <c15:sqref>Sheet1!$A$1:$A$23</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$A$2:$A$7,Sheet1!$A$11:$A$16,Sheet1!$A$19:$A$20)</c:f>
+              <c:f>(Sheet1!$A$2:$A$7,Sheet1!$A$11:$A$19,Sheet1!$A$22:$A$23)</c:f>
               <c:strCache>
-                <c:ptCount val="14"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>Raspberry Pi Model B+</c:v>
                 </c:pt>
@@ -481,9 +544,18 @@
                   <c:v>32Gb SD Card</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>Node Casing</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Battery</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Xbee</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>Weller WES51 Soldering Station</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>Female to Female Breadboard Wire</c:v>
                 </c:pt>
               </c:strCache>
@@ -494,14 +566,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$D$2:$D$20</c15:sqref>
+                    <c15:sqref>Sheet1!$D$2:$D$23</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$D$3:$D$8,Sheet1!$D$12:$D$17,Sheet1!$D$20)</c:f>
+              <c:f>(Sheet1!$D$3:$D$8,Sheet1!$D$12:$D$20,Sheet1!$D$23)</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>119.85000000000001</c:v>
                 </c:pt>
@@ -532,7 +604,16 @@
                 <c:pt idx="10">
                   <c:v>15.69</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>40</c:v>
+                </c:pt>
                 <c:pt idx="12">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>6.82</c:v>
                 </c:pt>
               </c:numCache>
@@ -574,7 +655,11 @@
                   <c15:bubble3D val="0"/>
                 </c15:categoryFilterException>
                 <c15:categoryFilterException>
-                  <c15:sqref>Sheet1!$D$19</c15:sqref>
+                  <c15:sqref>Sheet1!$D$21</c15:sqref>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+                <c15:categoryFilterException>
+                  <c15:sqref>Sheet1!$D$22</c15:sqref>
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:solidFill>
                       <a:schemeClr val="accent6">
@@ -589,7 +674,6 @@
                     </a:ln>
                     <a:effectLst/>
                   </c15:spPr>
-                  <c15:bubble3D val="0"/>
                 </c15:categoryFilterException>
               </c15:categoryFilterExceptions>
             </c:ext>
@@ -851,18 +935,62 @@
               <a:effectLst/>
             </c:spPr>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Sheet1!$A$10:$A$16</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>Sheet1!$A$11:$A$16</c:f>
+              <c:f>Sheet1!$A$11:$A$19</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>NVIDIA Jetson tk1</c:v>
                 </c:pt>
@@ -880,49 +1008,56 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>32Gb SD Card</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Node Casing</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Battery</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Xbee</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Sheet1!$B$10:$B$16</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>Sheet1!$B$11:$B$16</c:f>
+              <c:f>Sheet1!$D$11:$D$19</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>192.99</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>39.950000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>400.57</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>19.989999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>12.95</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>15.69</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:categoryFilterExceptions/>
-            </c:ext>
-          </c:extLst>
+          <c:extLst/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1030,20 +1165,102 @@
                     <a:effectLst/>
                   </c:spPr>
                 </c:dPt>
+                <c:dPt>
+                  <c:idx val="6"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="7"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="8"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="9"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent4">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="10"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent5">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
                 <c:cat>
                   <c:strRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:fullRef>
-                          <c15:sqref>Sheet1!$A$10:$A$16</c15:sqref>
-                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$A$11:$A$16</c15:sqref>
+                          <c15:sqref>Sheet1!$A$11:$A$19</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="9"/>
                       <c:pt idx="0">
                         <c:v>NVIDIA Jetson tk1</c:v>
                       </c:pt>
@@ -1061,6 +1278,15 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>32Gb SD Card</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Node Casing</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Battery</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Xbee</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1069,43 +1295,48 @@
                   <c:numRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:fullRef>
-                          <c15:sqref>Sheet1!$C$10:$C$16</c15:sqref>
-                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$C$11:$C$16</c15:sqref>
+                          <c15:sqref>Sheet1!$C$10:$C$20</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="11"/>
                       <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
                         <c:v>192.99</c:v>
                       </c:pt>
-                      <c:pt idx="1">
+                      <c:pt idx="2">
                         <c:v>39.950000000000003</c:v>
                       </c:pt>
-                      <c:pt idx="2">
+                      <c:pt idx="3">
                         <c:v>400.57</c:v>
                       </c:pt>
-                      <c:pt idx="3">
+                      <c:pt idx="4">
                         <c:v>19.989999999999998</c:v>
                       </c:pt>
-                      <c:pt idx="4">
+                      <c:pt idx="5">
                         <c:v>12.95</c:v>
                       </c:pt>
-                      <c:pt idx="5">
+                      <c:pt idx="6">
                         <c:v>15.69</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>50</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
-                  <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                    <c15:categoryFilterExceptions/>
-                  </c:ext>
-                </c:extLst>
+                <c:extLst/>
               </c15:ser>
             </c15:filteredPieSeries>
             <c15:filteredPieSeries>
@@ -1202,20 +1433,102 @@
                     <a:effectLst/>
                   </c:spPr>
                 </c:dPt>
+                <c:dPt>
+                  <c:idx val="6"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="7"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="8"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="9"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent4">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="10"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent5">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="19050">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:dPt>
                 <c:cat>
                   <c:strRef>
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:fullRef>
-                          <c15:sqref>Sheet1!$A$10:$A$16</c15:sqref>
-                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$A$11:$A$16</c15:sqref>
+                          <c15:sqref>Sheet1!$A$11:$A$19</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="9"/>
                       <c:pt idx="0">
                         <c:v>NVIDIA Jetson tk1</c:v>
                       </c:pt>
@@ -1233,6 +1546,15 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>32Gb SD Card</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Node Casing</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Battery</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Xbee</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1241,43 +1563,48 @@
                   <c:numRef>
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:fullRef>
-                          <c15:sqref>Sheet1!$D$10:$D$16</c15:sqref>
-                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$D$11:$D$16</c15:sqref>
+                          <c15:sqref>Sheet1!$D$10:$D$20</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="11"/>
                       <c:pt idx="0">
+                        <c:v>682.1400000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
                         <c:v>192.99</c:v>
                       </c:pt>
-                      <c:pt idx="1">
+                      <c:pt idx="2">
                         <c:v>39.950000000000003</c:v>
                       </c:pt>
-                      <c:pt idx="2">
+                      <c:pt idx="3">
                         <c:v>400.57</c:v>
                       </c:pt>
-                      <c:pt idx="3">
+                      <c:pt idx="4">
                         <c:v>19.989999999999998</c:v>
                       </c:pt>
-                      <c:pt idx="4">
+                      <c:pt idx="5">
                         <c:v>12.95</c:v>
                       </c:pt>
-                      <c:pt idx="5">
+                      <c:pt idx="6">
                         <c:v>15.69</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>50</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
-                  <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                    <c15:categoryFilterExceptions/>
-                  </c:ext>
-                </c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
               </c15:ser>
             </c15:filteredPieSeries>
           </c:ext>
@@ -2490,7 +2817,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2514,13 +2841,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2806,10 +3133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:D16"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2853,8 +3180,8 @@
         <v>119.85000000000001</v>
       </c>
       <c r="F2" s="2">
-        <f>SUM(D2:D196)</f>
-        <v>1899.0700000000002</v>
+        <f>SUM(D2:D199)</f>
+        <v>2029.0700000000002</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2868,7 +3195,7 @@
         <v>39.950000000000003</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D24" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D19" si="0">B3*C3</f>
         <v>119.85000000000001</v>
       </c>
     </row>
@@ -3041,55 +3368,99 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D17" s="1"/>
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>40</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>40</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" s="1">
-        <v>82.5</v>
+        <v>50</v>
       </c>
       <c r="D19" s="1">
-        <f>B19*C19</f>
-        <v>82.5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20" s="1">
-        <v>3.41</v>
-      </c>
-      <c r="D20" s="1">
-        <f>B20*C20</f>
-        <v>6.82</v>
-      </c>
+      <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D22" s="1"/>
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1">
+        <v>82.5</v>
+      </c>
+      <c r="D22" s="1">
+        <f>B22*C22</f>
+        <v>82.5</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D23" s="1"/>
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3.41</v>
+      </c>
+      <c r="D23" s="1">
+        <f>B23*C23</f>
+        <v>6.82</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>